<commit_message>
- Moved `nFile` out from pre-init loading stage due its high priority before loading extensions - Moved some server properties fields from `AppInitializer`to the `AppContext` - `nFile` init will be done follow by extension extraction during the `AppInitializer` being initialized - Moved color palette used by the neon start/end title to a separated class - Added a log when the database connect has been successfully established - Added a `NeonAPI` class which expose all the required function to the extension - Updated imports - Updated `AppContext` & `AppInitializer` run order - Removed older folder init function - Added missing nms mapping - Updated pom for `Neon-Database-Extension` - Updated extension loading will be run after the extraction
Signed-off-by: ICitiesz <69842262+ICitiesz@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Neon-Kotlin/src/main/resources/application/reflection/nms-mappings.xlsx
+++ b/Neon-Kotlin/src/main/resources/application/reflection/nms-mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal-Projects\Minecraft Development\Plugin\Neon\Neon-Kotlin\src\main\resources\application\reflection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39896822-EA69-42DF-8FFC-6F24A60D9F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C7E97-5BF5-4960-AE1B-5F185F170FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16425" yWindow="1455" windowWidth="21600" windowHeight="11295" xr2:uid="{C9B73305-C619-406D-9F72-FC33B9D3146E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9B73305-C619-406D-9F72-FC33B9D3146E}"/>
   </bookViews>
   <sheets>
     <sheet name="field" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="121">
   <si>
     <t>Object Name</t>
   </si>
@@ -393,13 +393,22 @@
   </si>
   <si>
     <t>1.19.3, 1.19.4, 1.20, 1.20.1, 1.20.2</t>
+  </si>
+  <si>
+    <t>RegistryEntryToggleState</t>
+  </si>
+  <si>
+    <t>bL</t>
+  </si>
+  <si>
+    <t>ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +420,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -803,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D307A551-2AD1-41CC-BE91-5D743987FF8D}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1293,41 @@
         <v>73</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>